<commit_message>
Excelfix - Fehlende Spalte in Periode 4 gefixt, daher Excel von Periode 4 verwenden. Excel von Periode 3 ist unfixed, aufgrund von nachvollziehbarkeit...
</commit_message>
<xml_diff>
--- a/Doc/IbsysExcelTool_Periode4.xlsx
+++ b/Doc/IbsysExcelTool_Periode4.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Entwicklung\Repo\Alugurke\Doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7308"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Produktionsprogramm" sheetId="1" r:id="rId1"/>
@@ -14,9 +19,9 @@
     <sheet name="Kapazitätsplan" sheetId="7" r:id="rId5"/>
     <sheet name="Tabelle1" sheetId="8" state="hidden" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="152511"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -254,8 +259,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,6 +433,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -436,21 +444,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -464,8 +457,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -739,30 +744,30 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:6">
-      <c r="B2" s="26" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="26"/>
-    </row>
-    <row r="3" spans="2:6" ht="15" thickBot="1"/>
-    <row r="4" spans="2:6">
+      <c r="C2" s="27"/>
+    </row>
+    <row r="3" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
         <v>0</v>
       </c>
@@ -779,7 +784,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>1</v>
       </c>
@@ -796,7 +801,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
@@ -813,12 +818,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15" thickBot="1">
+    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="12">
-        <v>200</v>
+        <v>50</v>
       </c>
       <c r="D7" s="12">
         <v>50</v>
@@ -839,32 +844,32 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="3.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="3.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="3.140625" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="2.88671875" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="19.44140625" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="17.7" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:15" ht="46.2" customHeight="1">
+    <row r="1" spans="2:15" ht="17.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -892,7 +897,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -900,11 +905,11 @@
         <f>Produktionsprogramm!C5</f>
         <v>200</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="D3" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="6">
         <v>20</v>
       </c>
@@ -930,7 +935,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -957,7 +962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -997,11 +1002,11 @@
         <v>7</v>
       </c>
       <c r="O5" s="9">
-        <f>IF((C5+G5-I5-K5-M5)&lt;0,0,C5+G5-I5-K5-M5)</f>
+        <f>IF((C5+E5+G5-I5-K5-M5)&lt;0,0,C5+E5+G5-I5-K5-M5)</f>
         <v>123.33333333333333</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
@@ -1040,11 +1045,11 @@
         <v>7</v>
       </c>
       <c r="O6" s="9">
-        <f t="shared" ref="O6:O18" si="1">IF((C6+G6-I6-K6-M6)&lt;0,0,C6+G6-I6-K6-M6)</f>
+        <f t="shared" ref="O6:O18" si="1">IF((C6+E6+G6-I6-K6-M6)&lt;0,0,C6+E6+G6-I6-K6-M6)</f>
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:15">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="6" t="s">
@@ -1075,7 +1080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1119,7 +1124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1150,7 +1155,7 @@
       <c r="J9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="38">
+      <c r="K9" s="26">
         <f>10/3</f>
         <v>3.3333333333333335</v>
       </c>
@@ -1169,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>11</v>
       </c>
@@ -1212,7 +1217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
       <c r="D11" s="6" t="s">
@@ -1243,7 +1248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>12</v>
       </c>
@@ -1286,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>13</v>
       </c>
@@ -1329,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>14</v>
       </c>
@@ -1372,7 +1377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
       <c r="D15" s="6" t="s">
@@ -1403,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
@@ -1446,7 +1451,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>16</v>
       </c>
@@ -1489,7 +1494,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="15" thickBot="1">
+    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>17</v>
       </c>
@@ -1532,13 +1537,13 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="28" t="s">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1551,32 +1556,32 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="O5" sqref="O5:O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="3.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="3.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="3.140625" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="2.88671875" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="19.44140625" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="17.7" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:15" ht="46.2" customHeight="1">
+    <row r="1" spans="2:15" ht="17.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -1604,7 +1609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
@@ -1612,11 +1617,11 @@
         <f>Produktionsprogramm!C6</f>
         <v>100</v>
       </c>
-      <c r="D3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+      <c r="D3" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="25">
         <v>20</v>
       </c>
@@ -1642,7 +1647,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:15">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1666,7 +1671,7 @@
       </c>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
@@ -1706,11 +1711,11 @@
         <v>7</v>
       </c>
       <c r="O5" s="9">
-        <f>IF((C5+G5-I5-K5-M5)&lt;0,0,C5+G5-I5-K5-M5)</f>
+        <f>IF((C5+E5+G5-I5-K5-M5)&lt;0,0,C5+E5+G5-I5-K5-M5)</f>
         <v>23.333333333333329</v>
       </c>
     </row>
-    <row r="6" spans="2:15">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>37</v>
       </c>
@@ -1749,11 +1754,11 @@
         <v>7</v>
       </c>
       <c r="O6" s="9">
-        <f t="shared" ref="O6:O18" si="0">IF((C6+G6-I6-K6-M6)&lt;0,0,C6+G6-I6-K6-M6)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15">
+        <f t="shared" ref="O6:O18" si="0">IF((C6+E6+G6-I6-K6-M6)&lt;0,0,C6+E6+G6-I6-K6-M6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="6" t="s">
@@ -1779,9 +1784,12 @@
       <c r="N7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="9"/>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="O7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
@@ -1825,7 +1833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
@@ -1875,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
@@ -1911,7 +1919,7 @@
       <c r="L10" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="M10" s="38">
+      <c r="M10" s="26">
         <v>10</v>
       </c>
       <c r="N10" s="6" t="s">
@@ -1922,7 +1930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
       <c r="D11" s="6" t="s">
@@ -1948,9 +1956,12 @@
       <c r="N11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="9"/>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="O11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>39</v>
       </c>
@@ -1993,7 +2004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>40</v>
       </c>
@@ -2036,7 +2047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>41</v>
       </c>
@@ -2083,7 +2094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
       <c r="D15" s="6" t="s">
@@ -2109,9 +2120,12 @@
       <c r="N15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O15" s="9"/>
-    </row>
-    <row r="16" spans="2:15">
+      <c r="O15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>42</v>
       </c>
@@ -2155,10 +2169,10 @@
       </c>
       <c r="O16" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>43</v>
       </c>
@@ -2198,10 +2212,10 @@
       </c>
       <c r="O17" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:15" ht="15" thickBot="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>44</v>
       </c>
@@ -2245,23 +2259,23 @@
       </c>
       <c r="O18" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="28" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-    </row>
-    <row r="28" spans="2:15">
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G28" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="2:15">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.25">
       <c r="G29" t="s">
         <v>73</v>
       </c>
@@ -2277,32 +2291,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.5546875" customWidth="1"/>
-    <col min="4" max="4" width="3.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" customWidth="1"/>
-    <col min="6" max="6" width="3.109375" customWidth="1"/>
-    <col min="7" max="7" width="24.33203125" customWidth="1"/>
-    <col min="8" max="8" width="3.109375" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="3.140625" customWidth="1"/>
+    <col min="7" max="7" width="24.28515625" customWidth="1"/>
+    <col min="8" max="8" width="3.140625" customWidth="1"/>
     <col min="9" max="9" width="18" customWidth="1"/>
-    <col min="10" max="10" width="2.88671875" customWidth="1"/>
+    <col min="10" max="10" width="2.85546875" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="3" customWidth="1"/>
-    <col min="13" max="13" width="14.6640625" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="14" width="4" customWidth="1"/>
-    <col min="15" max="15" width="19.44140625" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="17.7" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:15" ht="46.2" customHeight="1">
+    <row r="1" spans="2:15" ht="17.649999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:15" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
       <c r="C2" s="2" t="s">
         <v>18</v>
@@ -2330,19 +2344,19 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:15">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C3" s="6">
         <f>Produktionsprogramm!C7</f>
-        <v>200</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
+        <v>50</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
       <c r="G3" s="25">
         <v>20</v>
       </c>
@@ -2369,10 +2383,10 @@
       </c>
       <c r="O3" s="9">
         <f>IF((C3+G3-I3-K3-M3)&lt;0,0,C3+G3-I3-K3-M3)</f>
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -2396,13 +2410,13 @@
       </c>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="2:15">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C5" s="8">
         <f>O$3</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>5</v>
@@ -2436,17 +2450,17 @@
         <v>7</v>
       </c>
       <c r="O5" s="9">
-        <f>IF((C5+G5-I5-K5-M5)&lt;0,0,C5+G5-I5-K5-M5)</f>
-        <v>93.333333333333329</v>
-      </c>
-    </row>
-    <row r="6" spans="2:15">
+        <f>IF((C5+E5+G5-I5-K5-M5)&lt;0,0,C5+E5+G5-I5-K5-M5)</f>
+        <v>83.333333333333329</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="8">
         <f>O$3</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>5</v>
@@ -2479,11 +2493,11 @@
         <v>7</v>
       </c>
       <c r="O6" s="9">
-        <f t="shared" ref="O6:O18" si="0">IF((C6+G6-I6-K6-M6)&lt;0,0,C6+G6-I6-K6-M6)</f>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15">
+        <f t="shared" ref="O6:O18" si="0">IF((C6+E6+G6-I6-K6-M6)&lt;0,0,C6+E6+G6-I6-K6-M6)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="8"/>
       <c r="D7" s="6" t="s">
@@ -2509,15 +2523,18 @@
       <c r="N7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O7" s="9"/>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="O7" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="8">
         <f>O$6</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>5</v>
@@ -2552,16 +2569,16 @@
       </c>
       <c r="O8" s="9">
         <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="8">
         <f t="shared" ref="C9:C10" si="1">O$6</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>5</v>
@@ -2602,16 +2619,16 @@
       </c>
       <c r="O9" s="9">
         <f t="shared" si="0"/>
-        <v>15.000000000000005</v>
-      </c>
-    </row>
-    <row r="10" spans="2:15">
+        <v>5.0000000000000036</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C10" s="8">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>5</v>
@@ -2645,10 +2662,10 @@
       </c>
       <c r="O10" s="9">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="2:15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
       <c r="C11" s="8"/>
       <c r="D11" s="6" t="s">
@@ -2674,15 +2691,18 @@
       <c r="N11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O11" s="9"/>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="O11" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C12" s="8">
         <f>O$10</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>5</v>
@@ -2716,16 +2736,16 @@
       </c>
       <c r="O12" s="9">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="8">
         <f t="shared" ref="C13:C14" si="3">O$10</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>5</v>
@@ -2759,16 +2779,16 @@
       </c>
       <c r="O13" s="9">
         <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" s="5" t="s">
         <v>32</v>
       </c>
       <c r="C14" s="8">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>5</v>
@@ -2805,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
       <c r="C15" s="8"/>
       <c r="D15" s="6" t="s">
@@ -2831,9 +2851,12 @@
       <c r="N15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="O15" s="9"/>
-    </row>
-    <row r="16" spans="2:15">
+      <c r="O15" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>33</v>
       </c>
@@ -2878,7 +2901,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:15">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>34</v>
       </c>
@@ -2921,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:15" ht="15" thickBot="1">
+    <row r="18" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="10" t="s">
         <v>35</v>
       </c>
@@ -2964,13 +2987,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:15">
-      <c r="B20" s="28" t="s">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2983,59 +3006,59 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
-    <col min="4" max="4" width="5.109375" customWidth="1"/>
-    <col min="5" max="5" width="8.33203125" customWidth="1"/>
-    <col min="6" max="20" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.140625" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" customWidth="1"/>
+    <col min="6" max="20" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" ht="15" thickBot="1"/>
-    <row r="3" spans="2:20">
+    <row r="2" spans="2:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C3" s="17"/>
-      <c r="D3" s="36" t="s">
+      <c r="D3" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="34"/>
-      <c r="R3" s="34"/>
-      <c r="S3" s="34"/>
-      <c r="T3" s="35"/>
-    </row>
-    <row r="4" spans="2:20">
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="30"/>
+      <c r="T3" s="31"/>
+    </row>
+    <row r="4" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B4" s="18" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="19"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
       <c r="F4" s="6">
         <v>1</v>
       </c>
@@ -3082,8 +3105,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:20">
-      <c r="B5" s="33" t="s">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B5" s="36" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -3118,8 +3141,8 @@
       <c r="S5" s="6"/>
       <c r="T5" s="15"/>
     </row>
-    <row r="6" spans="2:20">
-      <c r="B6" s="33"/>
+    <row r="6" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B6" s="36"/>
       <c r="C6" s="19" t="s">
         <v>65</v>
       </c>
@@ -3152,8 +3175,8 @@
       <c r="S6" s="6"/>
       <c r="T6" s="15"/>
     </row>
-    <row r="7" spans="2:20">
-      <c r="B7" s="33"/>
+    <row r="7" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B7" s="36"/>
       <c r="C7" s="19" t="s">
         <v>66</v>
       </c>
@@ -3162,7 +3185,7 @@
       </c>
       <c r="E7" s="8">
         <f>Disposition_P3!O12</f>
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -3175,19 +3198,19 @@
       <c r="N7" s="6"/>
       <c r="O7" s="8">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="P7" s="8">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="15"/>
     </row>
-    <row r="8" spans="2:20">
-      <c r="B8" s="33" t="s">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B8" s="36" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="19" t="s">
@@ -3222,8 +3245,8 @@
       <c r="S8" s="6"/>
       <c r="T8" s="15"/>
     </row>
-    <row r="9" spans="2:20">
-      <c r="B9" s="33"/>
+    <row r="9" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B9" s="36"/>
       <c r="C9" s="19" t="s">
         <v>65</v>
       </c>
@@ -3232,7 +3255,7 @@
       </c>
       <c r="E9" s="8">
         <f>Disposition_P2!O16</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -3245,19 +3268,19 @@
       <c r="N9" s="6"/>
       <c r="O9" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="P9" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="15"/>
     </row>
-    <row r="10" spans="2:20">
-      <c r="B10" s="33"/>
+    <row r="10" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B10" s="36"/>
       <c r="C10" s="19" t="s">
         <v>66</v>
       </c>
@@ -3290,8 +3313,8 @@
       <c r="S10" s="6"/>
       <c r="T10" s="15"/>
     </row>
-    <row r="11" spans="2:20">
-      <c r="B11" s="33" t="s">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B11" s="36" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="19" t="s">
@@ -3335,8 +3358,8 @@
       <c r="S11" s="6"/>
       <c r="T11" s="15"/>
     </row>
-    <row r="12" spans="2:20">
-      <c r="B12" s="33"/>
+    <row r="12" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B12" s="36"/>
       <c r="C12" s="19" t="s">
         <v>65</v>
       </c>
@@ -3378,8 +3401,8 @@
       <c r="S12" s="6"/>
       <c r="T12" s="15"/>
     </row>
-    <row r="13" spans="2:20">
-      <c r="B13" s="33"/>
+    <row r="13" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B13" s="36"/>
       <c r="C13" s="19" t="s">
         <v>66</v>
       </c>
@@ -3388,7 +3411,7 @@
       </c>
       <c r="E13" s="8">
         <f>Disposition_P3!O13</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
@@ -3398,31 +3421,31 @@
       <c r="K13" s="6"/>
       <c r="L13" s="8">
         <f t="shared" si="2"/>
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="M13" s="8">
         <f>2*E13</f>
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="N13" s="8">
         <f t="shared" si="3"/>
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="8">
         <f t="shared" si="4"/>
-        <v>210</v>
+        <v>180</v>
       </c>
       <c r="R13" s="8">
         <f t="shared" si="5"/>
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="S13" s="6"/>
       <c r="T13" s="15"/>
     </row>
-    <row r="14" spans="2:20">
-      <c r="B14" s="33" t="s">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B14" s="36" t="s">
         <v>49</v>
       </c>
       <c r="C14" s="19" t="s">
@@ -3466,8 +3489,8 @@
       <c r="S14" s="6"/>
       <c r="T14" s="15"/>
     </row>
-    <row r="15" spans="2:20">
-      <c r="B15" s="33"/>
+    <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B15" s="36"/>
       <c r="C15" s="19" t="s">
         <v>65</v>
       </c>
@@ -3476,7 +3499,7 @@
       </c>
       <c r="E15" s="8">
         <f>Disposition_P2!O17</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
@@ -3486,31 +3509,31 @@
       <c r="K15" s="6"/>
       <c r="L15" s="8">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="M15" s="8">
         <f>2*E15</f>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="N15" s="8">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="8">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="R15" s="8">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="S15" s="6"/>
       <c r="T15" s="15"/>
     </row>
-    <row r="16" spans="2:20">
-      <c r="B16" s="33"/>
+    <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" s="36"/>
       <c r="C16" s="19" t="s">
         <v>66</v>
       </c>
@@ -3552,7 +3575,7 @@
       <c r="S16" s="6"/>
       <c r="T16" s="15"/>
     </row>
-    <row r="17" spans="2:20">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
         <v>50</v>
       </c>
@@ -3564,7 +3587,7 @@
       </c>
       <c r="E17" s="8">
         <f>Disposition_P1!O8+Disposition_P2!O8+Disposition_P3!O8</f>
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -3573,7 +3596,7 @@
       <c r="J17" s="6"/>
       <c r="K17" s="8">
         <f>2*E17</f>
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
@@ -3584,11 +3607,11 @@
       <c r="R17" s="6"/>
       <c r="S17" s="8">
         <f>3*E17</f>
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="T17" s="15"/>
     </row>
-    <row r="18" spans="2:20">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="18" t="s">
         <v>51</v>
       </c>
@@ -3600,7 +3623,7 @@
       </c>
       <c r="E18" s="8">
         <f>Disposition_P1!O9+Disposition_P2!O9+Disposition_P3!O9</f>
-        <v>15.000000000000005</v>
+        <v>5.0000000000000036</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -3618,11 +3641,11 @@
       <c r="S18" s="6"/>
       <c r="T18" s="21">
         <f>3*E18</f>
-        <v>45.000000000000014</v>
-      </c>
-    </row>
-    <row r="19" spans="2:20">
-      <c r="B19" s="33" t="s">
+        <v>15.000000000000011</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B19" s="36" t="s">
         <v>52</v>
       </c>
       <c r="C19" s="19" t="s">
@@ -3663,8 +3686,8 @@
       <c r="S19" s="6"/>
       <c r="T19" s="15"/>
     </row>
-    <row r="20" spans="2:20">
-      <c r="B20" s="33"/>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B20" s="36"/>
       <c r="C20" s="19" t="s">
         <v>65</v>
       </c>
@@ -3673,7 +3696,7 @@
       </c>
       <c r="E20" s="8">
         <f>Disposition_P2!O18</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -3682,19 +3705,19 @@
       <c r="J20" s="6"/>
       <c r="K20" s="8">
         <f>3*E20</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="L20" s="8">
         <f t="shared" ref="L20:L22" si="7">2*E20</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="M20" s="8">
         <f t="shared" ref="M20:M21" si="8">3*E20</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="N20" s="8">
         <f t="shared" ref="N20:N21" si="9">2*E20</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="O20" s="6"/>
       <c r="P20" s="6"/>
@@ -3703,8 +3726,8 @@
       <c r="S20" s="6"/>
       <c r="T20" s="15"/>
     </row>
-    <row r="21" spans="2:20">
-      <c r="B21" s="33"/>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B21" s="36"/>
       <c r="C21" s="19" t="s">
         <v>66</v>
       </c>
@@ -3743,7 +3766,7 @@
       <c r="S21" s="6"/>
       <c r="T21" s="15"/>
     </row>
-    <row r="22" spans="2:20">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
         <v>53</v>
       </c>
@@ -3755,7 +3778,7 @@
       </c>
       <c r="E22" s="8">
         <f>Disposition_P1!O5+Disposition_P2!O5+Disposition_P3!O5</f>
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -3765,7 +3788,7 @@
       <c r="K22" s="6"/>
       <c r="L22" s="8">
         <f t="shared" si="7"/>
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
@@ -3776,11 +3799,11 @@
       <c r="S22" s="6"/>
       <c r="T22" s="21">
         <f>3*E22</f>
-        <v>720</v>
-      </c>
-    </row>
-    <row r="23" spans="2:20">
-      <c r="B23" s="33" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B23" s="36" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="19" t="s">
@@ -3812,8 +3835,8 @@
       <c r="S23" s="6"/>
       <c r="T23" s="15"/>
     </row>
-    <row r="24" spans="2:20">
-      <c r="B24" s="33"/>
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B24" s="36"/>
       <c r="C24" s="19" t="s">
         <v>65</v>
       </c>
@@ -3843,8 +3866,8 @@
       <c r="S24" s="6"/>
       <c r="T24" s="15"/>
     </row>
-    <row r="25" spans="2:20">
-      <c r="B25" s="33"/>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B25" s="36"/>
       <c r="C25" s="19" t="s">
         <v>66</v>
       </c>
@@ -3874,8 +3897,8 @@
       <c r="S25" s="6"/>
       <c r="T25" s="15"/>
     </row>
-    <row r="26" spans="2:20">
-      <c r="B26" s="33" t="s">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B26" s="36" t="s">
         <v>55</v>
       </c>
       <c r="C26" s="19" t="s">
@@ -3907,8 +3930,8 @@
       <c r="S26" s="6"/>
       <c r="T26" s="15"/>
     </row>
-    <row r="27" spans="2:20">
-      <c r="B27" s="33"/>
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B27" s="36"/>
       <c r="C27" s="19" t="s">
         <v>65</v>
       </c>
@@ -3938,8 +3961,8 @@
       <c r="S27" s="6"/>
       <c r="T27" s="15"/>
     </row>
-    <row r="28" spans="2:20">
-      <c r="B28" s="33"/>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B28" s="36"/>
       <c r="C28" s="19" t="s">
         <v>66</v>
       </c>
@@ -3948,12 +3971,12 @@
       </c>
       <c r="E28" s="8">
         <f>Disposition_P3!O10</f>
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="F28" s="6"/>
       <c r="G28" s="8">
         <f>5*E28</f>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
@@ -3969,8 +3992,8 @@
       <c r="S28" s="6"/>
       <c r="T28" s="15"/>
     </row>
-    <row r="29" spans="2:20">
-      <c r="B29" s="33" t="s">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B29" s="36" t="s">
         <v>56</v>
       </c>
       <c r="C29" s="19" t="s">
@@ -4002,8 +4025,8 @@
       <c r="S29" s="6"/>
       <c r="T29" s="15"/>
     </row>
-    <row r="30" spans="2:20">
-      <c r="B30" s="33"/>
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B30" s="36"/>
       <c r="C30" s="19" t="s">
         <v>65</v>
       </c>
@@ -4033,8 +4056,8 @@
       <c r="S30" s="6"/>
       <c r="T30" s="15"/>
     </row>
-    <row r="31" spans="2:20">
-      <c r="B31" s="33"/>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B31" s="36"/>
       <c r="C31" s="19" t="s">
         <v>66</v>
       </c>
@@ -4043,13 +4066,13 @@
       </c>
       <c r="E31" s="8">
         <f>Disposition_P3!O6</f>
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="8">
         <f>6*E31</f>
-        <v>420</v>
+        <v>360</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="6"/>
@@ -4064,8 +4087,8 @@
       <c r="S31" s="6"/>
       <c r="T31" s="15"/>
     </row>
-    <row r="32" spans="2:20">
-      <c r="B32" s="33" t="s">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B32" s="36" t="s">
         <v>57</v>
       </c>
       <c r="C32" s="19" t="s">
@@ -4097,8 +4120,8 @@
       <c r="S32" s="6"/>
       <c r="T32" s="15"/>
     </row>
-    <row r="33" spans="2:22">
-      <c r="B33" s="33"/>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="36"/>
       <c r="C33" s="19" t="s">
         <v>65</v>
       </c>
@@ -4128,8 +4151,8 @@
       <c r="S33" s="6"/>
       <c r="T33" s="15"/>
     </row>
-    <row r="34" spans="2:22">
-      <c r="B34" s="33"/>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B34" s="36"/>
       <c r="C34" s="19" t="s">
         <v>66</v>
       </c>
@@ -4138,14 +4161,14 @@
       </c>
       <c r="E34" s="8">
         <f>Disposition_P3!O3</f>
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="8">
         <f>7*E34</f>
-        <v>630</v>
+        <v>0</v>
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6"/>
@@ -4163,28 +4186,28 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="35" spans="2:22">
-      <c r="B35" s="29" t="s">
+    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B35" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="35"/>
+      <c r="E35" s="35"/>
       <c r="F35" s="8">
         <f>SUM(F5:F34)</f>
         <v>0</v>
       </c>
       <c r="G35" s="8">
         <f t="shared" ref="G35:T35" si="10">SUM(G5:G34)</f>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="H35" s="8">
         <f t="shared" si="10"/>
-        <v>670</v>
+        <v>610</v>
       </c>
       <c r="I35" s="8">
         <f t="shared" si="10"/>
-        <v>1490</v>
+        <v>860</v>
       </c>
       <c r="J35" s="8">
         <f t="shared" si="10"/>
@@ -4192,52 +4215,52 @@
       </c>
       <c r="K35" s="8">
         <f t="shared" si="10"/>
-        <v>330</v>
+        <v>340</v>
       </c>
       <c r="L35" s="8">
         <f t="shared" si="10"/>
-        <v>820</v>
+        <v>900</v>
       </c>
       <c r="M35" s="8">
         <f t="shared" si="10"/>
-        <v>340</v>
+        <v>450</v>
       </c>
       <c r="N35" s="8">
         <f t="shared" si="10"/>
-        <v>460</v>
+        <v>600</v>
       </c>
       <c r="O35" s="8">
         <f t="shared" si="10"/>
-        <v>240</v>
+        <v>280</v>
       </c>
       <c r="P35" s="8">
         <f t="shared" si="10"/>
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="Q35" s="8">
         <f t="shared" si="10"/>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="R35" s="8">
         <f t="shared" si="10"/>
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="S35" s="8">
         <f t="shared" si="10"/>
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="T35" s="21">
         <f t="shared" si="10"/>
-        <v>765</v>
-      </c>
-    </row>
-    <row r="36" spans="2:22">
-      <c r="B36" s="29" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B36" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="35"/>
       <c r="F36" s="6">
         <f>IF(F23=0,0,20)+IF(F24=0,0,20)+IF(F25=0,0,20)</f>
         <v>0</v>
@@ -4252,34 +4275,34 @@
       </c>
       <c r="I36" s="6">
         <f>(IF(I32=0,0,1)+IF(I33=0,0,1)+IF(I34=0,0,1))*30</f>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="J36" s="6">
         <v>0</v>
       </c>
       <c r="K36" s="6">
         <f>(IF(K17=0,0,1)+IF(K19=0,0,1)+IF(K20=0,0,1)+IF(K21=0,0,1))*15</f>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="L36" s="6">
         <f>(IF(L11=0,0,1)+IF(L12=0,0,1)+IF(L13=0,0,1)+IF(L14=0,0,1)+IF(L15=0,0,1)+IF(L16=0,0,1)+IF(L19=0,0,1)+IF(L20=0,0,1)+IF(L21=0,0,1)+IF(L22=0,0,1))*20</f>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="M36" s="22">
         <f>(IF(M11=0,0,1)+IF(M12=0,0,1)+IF(M13=0,0,1)+IF(M14=0,0,1)+IF(M15=0,0,1)+IF(M16=0,0,1)+IF(M19=0,0,1)+IF(M20=0,0,1)+IF(M21=0,0,1))*15</f>
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="N36" s="22">
         <f>(IF(N11=0,0,1)+IF(N12=0,0,1)+IF(N13=0,0,1)+IF(N14=0,0,1)+IF(N15=0,0,1)+IF(N16=0,0,1)+IF(N19=0,0,1)+IF(N20=0,0,1)+IF(N21=0,0,1))*15</f>
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="O36" s="22">
         <f>(IF(O5=0,0,1)+IF(O6=0,0,1)+IF(O7=0,0,1)+IF(O8=0,0,1)+IF(O9=0,0,1)+IF(O10=0,0,1))*20</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="P36" s="22">
         <f>(IF(P5=0,0,1)+IF(P6=0,0,1)+IF(P7=0,0,1)+IF(P8=0,0,1)+IF(P9=0,0,1)+IF(P10=0,0,1))*20</f>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="Q36" s="22">
         <f>(IF(Q11=0,0,1)+IF(Q12=0,0,1)+IF(Q13=0,0,1)+IF(Q14=0,0,1)+IF(Q15=0,0,1)+IF(Q16=0,0,1))*0</f>
@@ -4298,13 +4321,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="2:22">
-      <c r="B37" s="29" t="s">
+    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B37" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="35"/>
       <c r="F37" s="6">
         <v>1080</v>
       </c>
@@ -4333,13 +4356,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="2:22">
-      <c r="B38" s="29" t="s">
+    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B38" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="35"/>
+      <c r="E38" s="35"/>
       <c r="F38" s="24"/>
       <c r="G38" s="24"/>
       <c r="H38" s="24"/>
@@ -4360,13 +4383,13 @@
       <c r="S38" s="24"/>
       <c r="T38" s="15"/>
     </row>
-    <row r="39" spans="2:22">
-      <c r="B39" s="29" t="s">
+    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B39" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="35"/>
       <c r="F39" s="6">
         <v>20</v>
       </c>
@@ -4399,28 +4422,28 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="2:22">
-      <c r="B40" s="29" t="s">
+    <row r="40" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B40" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
+      <c r="C40" s="35"/>
+      <c r="D40" s="35"/>
+      <c r="E40" s="35"/>
       <c r="F40" s="8">
         <f>SUM(F35:F39)</f>
         <v>1100</v>
       </c>
       <c r="G40" s="8">
         <f t="shared" ref="G40:T40" si="11">SUM(G35:G39)</f>
-        <v>610</v>
+        <v>560</v>
       </c>
       <c r="H40" s="8">
         <f t="shared" si="11"/>
-        <v>710</v>
+        <v>650</v>
       </c>
       <c r="I40" s="8">
         <f t="shared" si="11"/>
-        <v>2170</v>
+        <v>1510</v>
       </c>
       <c r="J40" s="8">
         <f t="shared" si="11"/>
@@ -4428,52 +4451,52 @@
       </c>
       <c r="K40" s="8">
         <f t="shared" si="11"/>
-        <v>360</v>
+        <v>385</v>
       </c>
       <c r="L40" s="8">
         <f t="shared" si="11"/>
-        <v>1400</v>
+        <v>1520</v>
       </c>
       <c r="M40" s="8">
         <f t="shared" si="11"/>
-        <v>1125</v>
+        <v>1265</v>
       </c>
       <c r="N40" s="8">
         <f t="shared" si="11"/>
-        <v>1005</v>
+        <v>1175</v>
       </c>
       <c r="O40" s="8">
         <f>SUM(O35:O39)</f>
-        <v>280</v>
+        <v>340</v>
       </c>
       <c r="P40" s="8">
         <f t="shared" si="11"/>
-        <v>390</v>
+        <v>440</v>
       </c>
       <c r="Q40" s="8">
         <f t="shared" si="11"/>
-        <v>360</v>
+        <v>480</v>
       </c>
       <c r="R40" s="8">
         <f t="shared" si="11"/>
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="S40" s="8">
         <f t="shared" si="11"/>
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="T40" s="21">
         <f t="shared" si="11"/>
-        <v>840</v>
-      </c>
-    </row>
-    <row r="41" spans="2:22" ht="15" thickBot="1">
-      <c r="B41" s="31" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="41" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
       <c r="F41" s="12">
         <f>IF((F40-2400)/5&lt;0,0,(F40-2400))</f>
         <v>0</v>
@@ -4535,7 +4558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:22">
+    <row r="43" spans="2:22" x14ac:dyDescent="0.25">
       <c r="F43" s="23">
         <v>1</v>
       </c>
@@ -4584,6 +4607,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B37:E37"/>
+    <mergeCell ref="B38:E38"/>
     <mergeCell ref="F3:T3"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="D3:D4"/>
@@ -4596,13 +4626,6 @@
     <mergeCell ref="B8:B10"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4610,12 +4633,12 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>